<commit_message>
AUT-887 Fix clients importing from file
</commit_message>
<xml_diff>
--- a/tara-admin-import/src/test/resources/import_files/client-with-all-fields.xlsx
+++ b/tara-admin-import/src/test/resources/import_files/client-with-all-fields.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16369AF7-25BF-43ED-B34D-B2ED40CCABCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD011BAA-66F0-42A6-B0F5-032A28ACE369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAS clients" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Institution name</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Example Institution</t>
+  </si>
+  <si>
+    <t>eIDAS RequesterID</t>
   </si>
 </sst>
 </file>
@@ -473,26 +476,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="11.140625" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="76.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="76.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="42.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,10 +536,13 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -576,7 +582,10 @@
       <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <v>1234</v>
+      </c>
+      <c r="O2" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>